<commit_message>
file refactoring for readability
</commit_message>
<xml_diff>
--- a/data_files/test.xlsx
+++ b/data_files/test.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,140 @@
       <c r="O1" t="inlineStr">
         <is>
           <t>Total sales</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>glop</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2" t="n">
+        <v>921321546465</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>4.73</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>15.23</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.71</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>15.93</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>23</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>glop</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G3" t="n">
+        <v>921321546465</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>4.73</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>15.23</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.71</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>15.93</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>23</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
edit item method implemented
</commit_message>
<xml_diff>
--- a/data_files/test.xlsx
+++ b/data_files/test.xlsx
@@ -1,26 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventory" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sales" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,16 +60,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -196,7 +236,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -231,7 +270,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -266,16 +304,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -397,403 +439,522 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="21.6" customWidth="1" style="2" min="9" max="9"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Item Desc</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Made in</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Size/ml-g-oz</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Bar Code</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Unit Price</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>45% Profit</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>Unit Price after profit</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>VAT</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>On hand qty</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>Sold qty</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>Total sales</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="3">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>lop</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>921321546465</v>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>10.5</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>4.73</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>15.23</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>0.71</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>15.93</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="3">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>glop</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>stock</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>eth</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D3" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>pcs</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F3" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G3" s="2" t="n">
         <v>921321546465</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H3" s="2" t="n">
         <v>10.5</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I3" s="2" t="inlineStr">
         <is>
           <t>4.73</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J3" s="2" t="inlineStr">
         <is>
           <t>15.23</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K3" s="2" t="inlineStr">
         <is>
           <t>0.71</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L3" s="2" t="inlineStr">
         <is>
           <t>15.93</t>
         </is>
       </c>
-      <c r="M2" t="n">
+      <c r="M3" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N3" s="2" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O3" s="2" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>glop</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>glplpp</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>stock</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>eth</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>pcs</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F4" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G4" s="2" t="n">
         <v>921321546465</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H4" s="2" t="n">
         <v>10.5</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I4" s="2" t="inlineStr">
         <is>
           <t>4.73</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J4" s="2" t="inlineStr">
         <is>
           <t>15.23</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K4" s="2" t="inlineStr">
         <is>
           <t>0.71</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L4" s="2" t="inlineStr">
         <is>
           <t>15.93</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="M4" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N4" s="2" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O4" s="2" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Item Desc</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Customer</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="3">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>lop</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>10.5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>105</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>lewi</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>2022-12-29 18:12:41</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="3">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>lop</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="2" t="n">
         <v>10.5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>lewi</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>2022-12-29 20:02:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="3">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>glop</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>lewi</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-03 12:32:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="3">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>glop</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>lewi</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-03 12:33:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="3">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>glop</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>lewi</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-03 12:36:35</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add item method implemented
</commit_message>
<xml_diff>
--- a/data_files/test.xlsx
+++ b/data_files/test.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
@@ -741,6 +741,69 @@
         <is>
           <t>0.00</t>
         </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>emp</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>951235648952</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>5.56</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>17.91</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>2.69</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>20.59</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sales method implementation and all sold inventory view and endpoint
</commit_message>
<xml_diff>
--- a/data_files/test.xlsx
+++ b/data_files/test.xlsx
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="M2" s="2" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="N2" s="2" t="inlineStr">
         <is>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="M4" s="2" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N4" s="2" t="inlineStr">
         <is>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="M5" s="2" t="n">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0</v>
@@ -819,7 +819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -992,6 +992,236 @@
       <c r="F6" s="2" t="inlineStr">
         <is>
           <t>2023-01-03 12:36:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>glplpp</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-05 20:43:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>lop</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>selome</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-05 20:43:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>lop</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>selome</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-07 17:06:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>lop</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>selome</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-07 17:09:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>lop</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>selome</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-07 17:10:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>lop</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>selome</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-07 17:10:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>emp</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>284.05</v>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>lewi</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-07 17:12:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>emp</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>284.05</v>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>lewi</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-07 17:13:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>emp</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>24.7</v>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Bogale</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-08 19:15:13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
templates modified to use basic html tags only, css changed to picocss instead of vanilla css, implemented modal.js to handle picocss based confirmation overlay
</commit_message>
<xml_diff>
--- a/data_files/test.xlsx
+++ b/data_files/test.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
@@ -541,7 +541,7 @@
     <row r="2" ht="15" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>lop</t>
+          <t>glop</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -551,13 +551,11 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>chn</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+          <t>eth</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
@@ -570,10 +568,8 @@
       <c r="G2" s="2" t="n">
         <v>921321546465</v>
       </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>10.5</t>
-        </is>
+      <c r="H2" s="2" t="n">
+        <v>10.5</v>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
@@ -596,7 +592,7 @@
         </is>
       </c>
       <c r="M2" s="2" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="N2" s="2" t="inlineStr">
         <is>
@@ -612,7 +608,7 @@
     <row r="3" ht="15" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>glop</t>
+          <t>glplpp</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -663,7 +659,7 @@
         </is>
       </c>
       <c r="M3" s="2" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
@@ -679,7 +675,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>glplpp</t>
+          <t>emp</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -689,11 +685,11 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>eth</t>
+          <t>chn</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
@@ -701,52 +697,48 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>921321546465</v>
+        <v>951235648952</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>10.5</v>
+        <v>12.35</v>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>4.73</t>
+          <t>5.56</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>15.23</t>
+          <t>17.91</t>
         </is>
       </c>
       <c r="K4" s="2" t="inlineStr">
         <is>
-          <t>0.71</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>15.93</t>
+          <t>20.59</t>
         </is>
       </c>
       <c r="M4" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="N4" s="2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="O4" s="2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+        <v>201</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>emp</t>
+          <t>opads</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -759,8 +751,10 @@
           <t>chn</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>10</v>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
@@ -773,36 +767,426 @@
       <c r="G5" s="2" t="n">
         <v>951235648952</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>12.35</v>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>12.35</t>
+        </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>5.56</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>17.91</t>
+          <t>17.40</t>
         </is>
       </c>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>2.69</t>
+          <t>2.61</t>
         </is>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>20.59</t>
+          <t>20.01</t>
         </is>
       </c>
       <c r="M5" s="2" t="n">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="O5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>lipbalm</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>lipstick</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>951235648952</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>4.68</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>15.08</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>2.26</t>
+        </is>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>17.34</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>asfafas</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>951235648952</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>5.56</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>17.91</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>2.69</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>20.59</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>247</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>etett</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>951235648952</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>454</v>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>204.30</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
+          <t>658.30</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>98.74</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>757.04</t>
+        </is>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>empkmkm</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>951235648952</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>12.32</v>
+      </c>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>5.54</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>17.86</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>2.68</t>
+        </is>
+      </c>
+      <c r="L9" s="2" t="inlineStr">
+        <is>
+          <t>20.54</t>
+        </is>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>emp</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>951235648952</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>5.56</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>17.91</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>2.69</t>
+        </is>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
+        <is>
+          <t>20.59</t>
+        </is>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>emp</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>lipstick</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>chn</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>951235648952</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>12.35</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>5.56</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>17.91</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2.69</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>20.59</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -819,7 +1203,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1222,6 +1606,58 @@
       <c r="F15" s="2" t="inlineStr">
         <is>
           <t>2023-01-08 19:15:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>opads</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>123.5</v>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>selome</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-19 15:56:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>asfafas</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>24.7</v>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>selome</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>2023-01-19 16:32:50</t>
         </is>
       </c>
     </row>

</xml_diff>